<commit_message>
added some fake data to the data
</commit_message>
<xml_diff>
--- a/data/fake_data.xlsx
+++ b/data/fake_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Question</t>
   </si>
@@ -96,16 +96,98 @@
   </si>
   <si>
     <t>AllTheLINKS666</t>
+  </si>
+  <si>
+    <t>I just love brussel sprouts. And this guy (http://mywholefoodlife.com/2014/07/14/smokey-roasted-brussel-sprouts/) is too! The recipe he uses calls for brussel sprouts, 1 large sweet potato, 2 tablespoons of coconut oil, s tablesppons of maple syrup, 1/2 teaspoon of chili powder, and 1/2 teaspoon of sea salt. ....The coconut oil really does it for me. It's just so fatty! (Whatevs about the maple syrup - YOLO.) What can I use instead of the 2 tablespoons of coconut oil???</t>
+  </si>
+  <si>
+    <t>maplesyrup&lt;333</t>
+  </si>
+  <si>
+    <t>Roasting</t>
+  </si>
+  <si>
+    <t>Coconut oil has a lot of unhealthy saturated fats, while olive oil is a healthier alternative with more unsaturated fats.</t>
+  </si>
+  <si>
+    <t>ilikehealthyfoods</t>
+  </si>
+  <si>
+    <t>Use 2 tablespoons of canola oil! It's less expensive than olive oil.</t>
+  </si>
+  <si>
+    <t>Bananas! Bananas! Don't you love banana bread?   4 ripe bananas,
+1 cup butter,
+2 cups sugar,
+2 large eggs,
+1/2 cup low-fat mayonaise,
+1/2 cup milk,
+1 teaspoon baking soda,
+3 cups all-purpose flour,
+1 teaspoon vanilla,
+1/2 teaspoons salt. But I'm lactose-intolerant. What can I do about the milk and the butter? Thank you!</t>
+  </si>
+  <si>
+    <t>ughMilkWhyDoYouHurtMeSo</t>
+  </si>
+  <si>
+    <t>Answer3</t>
+  </si>
+  <si>
+    <t>Answer3_Username</t>
+  </si>
+  <si>
+    <t>Answer3_Time</t>
+  </si>
+  <si>
+    <t>Answer3_Upvotes</t>
+  </si>
+  <si>
+    <t>Answer3_Downvotes</t>
+  </si>
+  <si>
+    <t>Nobody likes brussel sprouts. Make brownies.</t>
+  </si>
+  <si>
+    <t>downwithvegetables</t>
+  </si>
+  <si>
+    <t>11/16/2014  13:29:45 PM</t>
+  </si>
+  <si>
+    <t>11/16/2014  14:29:45 PM</t>
+  </si>
+  <si>
+    <t>11/16/2014  14:05:51 PM</t>
+  </si>
+  <si>
+    <t>Lactose_Intolerant</t>
+  </si>
+  <si>
+    <t>Use margarine and soy milk instead of dairy products. I keep kosher and often can't cook using dairy. Enjoy :)</t>
+  </si>
+  <si>
+    <t>separate_milk_and_eat</t>
+  </si>
+  <si>
+    <t>11/16/2014  14:38:06 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,9 +213,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -434,9 +520,10 @@
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1"/>
     <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +572,23 @@
       <c r="P1" t="s">
         <v>21</v>
       </c>
+      <c r="Q1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -537,7 +639,105 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="1">
+        <v>41959.613449074073</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="1">
+        <v>41959.628101851849</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="195" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>